<commit_message>
Aggiornato DocInteraz e TempiLavoro
</commit_message>
<xml_diff>
--- a/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_Gianluca.xlsx
+++ b/Documentazione/GDPRPrj_TempiLavoro/GDPRPrj_TempiLavoro_Gianluca.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F33C4E3-1088-40E8-B2B8-CAB834B66268}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -16,17 +17,23 @@
     <definedName name="Progetto">Foglio1!$B:$B</definedName>
     <definedName name="Tempo">Foglio1!$G:$G</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="14">
   <si>
     <t>Persona</t>
   </si>
@@ -65,12 +72,15 @@
   </si>
   <si>
     <t>XAMPP</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -125,17 +135,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="E1:I1048576" totalsRowShown="0">
-  <autoFilter ref="E1:I1048576"/>
-  <sortState ref="E2:I19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="E1:I1048576" totalsRowShown="0">
+  <autoFilter ref="E1:I1048576" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:I18">
     <sortCondition ref="H1:H1048576"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="3" name="Persona"/>
-    <tableColumn id="4" name="Progetto"/>
-    <tableColumn id="1" name="Attività"/>
-    <tableColumn id="2" name="Data"/>
-    <tableColumn id="5" name="Tempo (min)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Persona"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progetto"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Attività"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Data"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Tempo (min)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -403,11 +413,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,21 +664,49 @@
       </c>
     </row>
     <row r="15" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H15" t="s">
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1">
+        <v>43552</v>
+      </c>
+      <c r="I15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="1">
+        <v>43552</v>
+      </c>
+      <c r="I16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
         <v>8</v>
       </c>
-      <c r="I15">
-        <f>SUM(I2:I14)</f>
-        <v>710</v>
-      </c>
-    </row>
-    <row r="16" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>SUM(I4:I16)</f>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="1"/>
     </row>
   </sheetData>

</xml_diff>